<commit_message>
done with other labels display
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_(Pandian).xlsx
+++ b/Wave 5_React_Tracker_(Pandian).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Git URL:https://github.com/Pandiyan927/react_gmail_assignment</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,7 +502,12 @@
       <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
changes in excel sheet
</commit_message>
<xml_diff>
--- a/Wave 5_React_Tracker_(Pandian).xlsx
+++ b/Wave 5_React_Tracker_(Pandian).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>React Basics (Architecture, Concepts, Lifecycle)</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>24/08/2016</t>
+  </si>
+  <si>
+    <t>25/08/2016</t>
+  </si>
+  <si>
+    <t>not started</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -409,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -500,12 +509,70 @@
         <v>13</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>